<commit_message>
sample size table update
</commit_message>
<xml_diff>
--- a/doc/table.xlsx
+++ b/doc/table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t xml:space="preserve">Instruments</t>
   </si>
@@ -69,6 +69,15 @@
     <t xml:space="preserve">H3-0 DEDM</t>
   </si>
   <si>
+    <t xml:space="preserve">4.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">full beam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">H3-1 IN-2</t>
   </si>
   <si>
@@ -93,7 +102,7 @@
     <t xml:space="preserve">4.5-20</t>
   </si>
   <si>
-    <t xml:space="preserve">1х1</t>
+    <t xml:space="preserve">3x3</t>
   </si>
   <si>
     <t xml:space="preserve">M=2</t>
@@ -109,6 +118,9 @@
   </si>
   <si>
     <t xml:space="preserve">H3-4 Tensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5x5</t>
   </si>
   <si>
     <t xml:space="preserve">H3-5 TOF</t>
@@ -220,7 +232,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -298,13 +310,25 @@
       <c r="A6" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>11</v>
@@ -318,78 +342,87 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C12" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
m downgrade scan + ell
</commit_message>
<xml_diff>
--- a/doc/table.xlsx
+++ b/doc/table.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="89">
   <si>
     <t>Instruments</t>
   </si>
@@ -255,6 +255,39 @@
   </si>
   <si>
     <t>mono</t>
+  </si>
+  <si>
+    <t>straight</t>
+  </si>
+  <si>
+    <t>R = 800, L = 23</t>
+  </si>
+  <si>
+    <t>R = 900, L = 25</t>
+  </si>
+  <si>
+    <t>R = 100,L = 11</t>
+  </si>
+  <si>
+    <t>R = 800, L = 14</t>
+  </si>
+  <si>
+    <t>R = 600, L = 42</t>
+  </si>
+  <si>
+    <t>R = 900, L = 52</t>
+  </si>
+  <si>
+    <t>R = 700, L = 50 x 2</t>
+  </si>
+  <si>
+    <t>R = 240, L = 19, n = 12</t>
+  </si>
+  <si>
+    <t>R = 325, L = 22, n = 5</t>
+  </si>
+  <si>
+    <t>R = 950, L = 26, n = 2</t>
   </si>
 </sst>
 </file>
@@ -590,7 +623,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -664,6 +697,9 @@
       <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="J2" s="1" t="s">
         <v>74</v>
       </c>
@@ -690,6 +726,9 @@
       <c r="G3" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>68</v>
       </c>
@@ -719,6 +758,9 @@
       <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="K4" s="1" t="s">
         <v>69</v>
       </c>
@@ -736,6 +778,9 @@
       <c r="G5" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="J5" s="1" t="s">
         <v>73</v>
       </c>
@@ -768,6 +813,9 @@
       <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="J6" s="1" t="s">
         <v>43</v>
       </c>
@@ -800,6 +848,9 @@
       <c r="G7" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="J7" s="1" t="s">
         <v>47</v>
       </c>
@@ -832,6 +883,9 @@
       <c r="G8" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="J8" s="1" t="s">
         <v>46</v>
       </c>
@@ -864,6 +918,9 @@
       <c r="G9" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="J9" s="1" t="s">
         <v>48</v>
       </c>
@@ -896,6 +953,9 @@
       <c r="G10" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="H10" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="K10" s="1" t="s">
         <v>53</v>
       </c>
@@ -925,6 +985,9 @@
       <c r="G11" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="H11" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="J11" s="1" t="s">
         <v>49</v>
       </c>
@@ -957,6 +1020,9 @@
       <c r="G12" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="H12" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="K12" s="1" t="s">
         <v>56</v>
       </c>
@@ -974,6 +1040,9 @@
       <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="K13" s="1" t="s">
         <v>60</v>
       </c>
@@ -1000,6 +1069,9 @@
       <c r="G14" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="H14" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="K14" s="1" t="s">
         <v>63</v>
       </c>
@@ -1020,11 +1092,17 @@
       <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="F15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Revert "Revert "s bendes""
This reverts commit 313e4ab89df538d04cfdb8cd0c605e732411a198.
</commit_message>
<xml_diff>
--- a/doc/table.xlsx
+++ b/doc/table.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="97">
   <si>
     <t>Instruments</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>-n-</t>
+  </si>
+  <si>
+    <t>S бендер</t>
   </si>
 </sst>
 </file>
@@ -668,7 +671,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1109,7 +1112,7 @@
         <v>57</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1136,34 +1139,39 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" t="s">
+      <c r="A14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="F14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L14" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M14" s="7" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add HEC2 IN-2 script, only bender
</commit_message>
<xml_diff>
--- a/doc/table.xlsx
+++ b/doc/table.xlsx
@@ -218,12 +218,6 @@
     <t>14</t>
   </si>
   <si>
-    <t>30.8</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
     <t>39.8+10</t>
   </si>
   <si>
@@ -312,6 +306,12 @@
   </si>
   <si>
     <t>54(56.7)//36</t>
+  </si>
+  <si>
+    <t>30.8(22)</t>
+  </si>
+  <si>
+    <t>2.2(0.18-0.32)</t>
   </si>
 </sst>
 </file>
@@ -671,7 +671,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -687,7 +687,7 @@
     <col min="9" max="9" width="19.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="1" customWidth="1"/>
     <col min="13" max="13" width="29" style="1" customWidth="1"/>
     <col min="14" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
@@ -712,7 +712,7 @@
         <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>36</v>
@@ -749,11 +749,11 @@
         <v>39</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>63</v>
@@ -781,7 +781,7 @@
         <v>39</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -815,16 +815,16 @@
         <v>39</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -838,19 +838,19 @@
         <v>39</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -876,10 +876,10 @@
         <v>38</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>43</v>
@@ -914,7 +914,7 @@
         <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>47</v>
@@ -926,7 +926,7 @@
         <v>57</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -934,7 +934,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
@@ -943,7 +943,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>38</v>
@@ -952,10 +952,10 @@
         <v>39</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>46</v>
@@ -981,7 +981,7 @@
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>39</v>
@@ -990,7 +990,7 @@
         <v>38</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>48</v>
@@ -1002,7 +1002,7 @@
         <v>55</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1019,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>39</v>
@@ -1028,7 +1028,7 @@
         <v>38</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -1039,7 +1039,7 @@
         <v>45</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1065,7 +1065,7 @@
         <v>38</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>49</v>
@@ -1077,7 +1077,7 @@
         <v>59</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1103,7 +1103,7 @@
         <v>38</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>56</v>
@@ -1112,7 +1112,7 @@
         <v>57</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1126,7 +1126,7 @@
         <v>38</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>60</v>
@@ -1135,7 +1135,7 @@
         <v>61</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1161,18 +1161,18 @@
         <v>38</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1198,20 +1198,20 @@
         <v>38</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7" t="s">
         <v>50</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>